<commit_message>
feat: alibaba easyExcel 遍历数据样式
</commit_message>
<xml_diff>
--- a/springboot-test/src/main/resources/template/composite.xlsx
+++ b/springboot-test/src/main/resources/template/composite.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
   <si>
     <t>统计</t>
   </si>
@@ -53,15 +53,21 @@
   <si>
     <t>{.dataList.string}</t>
   </si>
+  <si>
+    <t>fadsfs</t>
+  </si>
+  <si>
+    <t>fdsafsaf</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
@@ -95,6 +101,22 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
@@ -104,6 +126,68 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -117,108 +201,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -239,25 +245,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -269,13 +401,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -287,73 +413,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -365,71 +425,32 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -446,18 +467,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -473,6 +483,30 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -507,26 +541,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -535,169 +556,175 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1056,7 +1083,7 @@
   <dimension ref="A1:F106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="5"/>
@@ -1069,7 +1096,7 @@
     <col min="7" max="7" width="13.4615384615385" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1079,17 +1106,19 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="4"/>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1"/>
       <c r="B3" s="2" t="s">
         <v>1</v>
@@ -1097,8 +1126,9 @@
       <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1"/>
       <c r="B4" s="2" t="s">
         <v>3</v>
@@ -1106,12 +1136,13 @@
       <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="D4" s="4"/>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="7"/>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
@@ -1125,15 +1156,15 @@
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="4:6">
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="7" t="s">
         <v>3</v>
       </c>
       <c r="F10" t="s">
@@ -1141,10 +1172,10 @@
       </c>
     </row>
     <row r="11" spans="4:6">
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F11" t="s">
@@ -1152,291 +1183,297 @@
       </c>
     </row>
     <row r="12" spans="4:5">
-      <c r="D12" s="6"/>
-      <c r="E12" s="7"/>
-    </row>
-    <row r="13" spans="4:5">
-      <c r="D13" s="6"/>
-      <c r="E13" s="7"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="9"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="9"/>
     </row>
     <row r="14" spans="4:4">
-      <c r="D14" s="6"/>
+      <c r="D14" s="8"/>
     </row>
     <row r="15" spans="4:4">
-      <c r="D15" s="6"/>
+      <c r="D15" s="8"/>
     </row>
     <row r="16" spans="4:4">
-      <c r="D16" s="6"/>
+      <c r="D16" s="8"/>
     </row>
     <row r="17" spans="4:4">
-      <c r="D17" s="6"/>
+      <c r="D17" s="8"/>
     </row>
     <row r="18" spans="4:4">
-      <c r="D18" s="6"/>
+      <c r="D18" s="8"/>
     </row>
     <row r="19" spans="4:4">
-      <c r="D19" s="6"/>
+      <c r="D19" s="8"/>
     </row>
     <row r="20" spans="4:4">
-      <c r="D20" s="6"/>
+      <c r="D20" s="8"/>
     </row>
     <row r="21" spans="4:4">
-      <c r="D21" s="6"/>
+      <c r="D21" s="8"/>
     </row>
     <row r="22" spans="4:4">
-      <c r="D22" s="6"/>
+      <c r="D22" s="8"/>
     </row>
     <row r="23" spans="4:4">
-      <c r="D23" s="6"/>
+      <c r="D23" s="8"/>
     </row>
     <row r="24" spans="4:4">
-      <c r="D24" s="6"/>
+      <c r="D24" s="8"/>
     </row>
     <row r="25" spans="4:4">
-      <c r="D25" s="6"/>
+      <c r="D25" s="8"/>
     </row>
     <row r="26" spans="4:4">
-      <c r="D26" s="6"/>
+      <c r="D26" s="8"/>
     </row>
     <row r="27" spans="4:4">
-      <c r="D27" s="6"/>
+      <c r="D27" s="8"/>
     </row>
     <row r="28" spans="4:4">
-      <c r="D28" s="6"/>
+      <c r="D28" s="8"/>
     </row>
     <row r="29" spans="4:4">
-      <c r="D29" s="6"/>
+      <c r="D29" s="8"/>
     </row>
     <row r="30" spans="4:4">
-      <c r="D30" s="6"/>
+      <c r="D30" s="8"/>
     </row>
     <row r="31" spans="4:4">
-      <c r="D31" s="6"/>
+      <c r="D31" s="8"/>
     </row>
     <row r="32" spans="4:4">
-      <c r="D32" s="6"/>
+      <c r="D32" s="8"/>
     </row>
     <row r="33" spans="4:4">
-      <c r="D33" s="6"/>
+      <c r="D33" s="8"/>
     </row>
     <row r="34" spans="4:4">
-      <c r="D34" s="6"/>
+      <c r="D34" s="8"/>
     </row>
     <row r="35" spans="4:4">
-      <c r="D35" s="6"/>
+      <c r="D35" s="8"/>
     </row>
     <row r="36" spans="4:4">
-      <c r="D36" s="6"/>
+      <c r="D36" s="8"/>
     </row>
     <row r="37" spans="4:4">
-      <c r="D37" s="6"/>
+      <c r="D37" s="8"/>
     </row>
     <row r="38" spans="4:4">
-      <c r="D38" s="6"/>
+      <c r="D38" s="8"/>
     </row>
     <row r="39" spans="4:4">
-      <c r="D39" s="6"/>
+      <c r="D39" s="8"/>
     </row>
     <row r="40" spans="4:4">
-      <c r="D40" s="6"/>
+      <c r="D40" s="8"/>
     </row>
     <row r="41" spans="4:4">
-      <c r="D41" s="6"/>
+      <c r="D41" s="8"/>
     </row>
     <row r="42" spans="4:4">
-      <c r="D42" s="6"/>
+      <c r="D42" s="8"/>
     </row>
     <row r="43" spans="4:4">
-      <c r="D43" s="6"/>
+      <c r="D43" s="8"/>
     </row>
     <row r="44" spans="4:4">
-      <c r="D44" s="6"/>
+      <c r="D44" s="8"/>
     </row>
     <row r="45" spans="4:4">
-      <c r="D45" s="6"/>
+      <c r="D45" s="8"/>
     </row>
     <row r="46" spans="4:4">
-      <c r="D46" s="6"/>
+      <c r="D46" s="8"/>
     </row>
     <row r="47" spans="4:4">
-      <c r="D47" s="6"/>
+      <c r="D47" s="8"/>
     </row>
     <row r="48" spans="4:4">
-      <c r="D48" s="6"/>
+      <c r="D48" s="8"/>
     </row>
     <row r="49" spans="4:4">
-      <c r="D49" s="6"/>
+      <c r="D49" s="8"/>
     </row>
     <row r="50" spans="4:4">
-      <c r="D50" s="6"/>
+      <c r="D50" s="8"/>
     </row>
     <row r="51" spans="4:4">
-      <c r="D51" s="6"/>
+      <c r="D51" s="8"/>
     </row>
     <row r="52" spans="4:4">
-      <c r="D52" s="6"/>
+      <c r="D52" s="8"/>
     </row>
     <row r="53" spans="4:4">
-      <c r="D53" s="6"/>
+      <c r="D53" s="8"/>
     </row>
     <row r="54" spans="4:4">
-      <c r="D54" s="6"/>
+      <c r="D54" s="8"/>
     </row>
     <row r="55" spans="4:4">
-      <c r="D55" s="6"/>
+      <c r="D55" s="8"/>
     </row>
     <row r="56" spans="4:4">
-      <c r="D56" s="6"/>
+      <c r="D56" s="8"/>
     </row>
     <row r="57" spans="4:4">
-      <c r="D57" s="6"/>
+      <c r="D57" s="8"/>
     </row>
     <row r="58" spans="4:4">
-      <c r="D58" s="6"/>
+      <c r="D58" s="8"/>
     </row>
     <row r="59" spans="4:4">
-      <c r="D59" s="6"/>
+      <c r="D59" s="8"/>
     </row>
     <row r="60" spans="4:4">
-      <c r="D60" s="6"/>
+      <c r="D60" s="8"/>
     </row>
     <row r="61" spans="4:4">
-      <c r="D61" s="6"/>
+      <c r="D61" s="8"/>
     </row>
     <row r="62" spans="4:4">
-      <c r="D62" s="6"/>
+      <c r="D62" s="8"/>
     </row>
     <row r="63" spans="4:4">
-      <c r="D63" s="6"/>
+      <c r="D63" s="8"/>
     </row>
     <row r="64" spans="4:4">
-      <c r="D64" s="6"/>
+      <c r="D64" s="8"/>
     </row>
     <row r="65" spans="4:4">
-      <c r="D65" s="6"/>
+      <c r="D65" s="8"/>
     </row>
     <row r="66" spans="4:4">
-      <c r="D66" s="6"/>
+      <c r="D66" s="8"/>
     </row>
     <row r="67" spans="4:4">
-      <c r="D67" s="6"/>
+      <c r="D67" s="8"/>
     </row>
     <row r="68" spans="4:4">
-      <c r="D68" s="6"/>
+      <c r="D68" s="8"/>
     </row>
     <row r="69" spans="4:4">
-      <c r="D69" s="6"/>
+      <c r="D69" s="8"/>
     </row>
     <row r="70" spans="4:4">
-      <c r="D70" s="6"/>
+      <c r="D70" s="8"/>
     </row>
     <row r="71" spans="4:4">
-      <c r="D71" s="6"/>
+      <c r="D71" s="8"/>
     </row>
     <row r="72" spans="4:4">
-      <c r="D72" s="6"/>
+      <c r="D72" s="8"/>
     </row>
     <row r="73" spans="4:4">
-      <c r="D73" s="6"/>
+      <c r="D73" s="8"/>
     </row>
     <row r="74" spans="4:4">
-      <c r="D74" s="6"/>
+      <c r="D74" s="8"/>
     </row>
     <row r="75" spans="4:4">
-      <c r="D75" s="6"/>
+      <c r="D75" s="8"/>
     </row>
     <row r="76" spans="4:4">
-      <c r="D76" s="6"/>
+      <c r="D76" s="8"/>
     </row>
     <row r="77" spans="4:4">
-      <c r="D77" s="6"/>
+      <c r="D77" s="8"/>
     </row>
     <row r="78" spans="4:4">
-      <c r="D78" s="6"/>
+      <c r="D78" s="8"/>
     </row>
     <row r="79" spans="4:4">
-      <c r="D79" s="6"/>
+      <c r="D79" s="8"/>
     </row>
     <row r="80" spans="4:4">
-      <c r="D80" s="6"/>
+      <c r="D80" s="8"/>
     </row>
     <row r="81" spans="4:4">
-      <c r="D81" s="6"/>
+      <c r="D81" s="8"/>
     </row>
     <row r="82" spans="4:4">
-      <c r="D82" s="6"/>
+      <c r="D82" s="8"/>
     </row>
     <row r="83" spans="4:4">
-      <c r="D83" s="6"/>
+      <c r="D83" s="8"/>
     </row>
     <row r="84" spans="4:4">
-      <c r="D84" s="6"/>
+      <c r="D84" s="8"/>
     </row>
     <row r="85" spans="4:4">
-      <c r="D85" s="6"/>
+      <c r="D85" s="8"/>
     </row>
     <row r="86" spans="4:4">
-      <c r="D86" s="6"/>
+      <c r="D86" s="8"/>
     </row>
     <row r="87" spans="4:4">
-      <c r="D87" s="6"/>
+      <c r="D87" s="8"/>
     </row>
     <row r="88" spans="4:4">
-      <c r="D88" s="6"/>
+      <c r="D88" s="8"/>
     </row>
     <row r="89" spans="4:4">
-      <c r="D89" s="6"/>
+      <c r="D89" s="8"/>
     </row>
     <row r="90" spans="4:4">
-      <c r="D90" s="6"/>
+      <c r="D90" s="8"/>
     </row>
     <row r="91" spans="4:4">
-      <c r="D91" s="6"/>
+      <c r="D91" s="8"/>
     </row>
     <row r="92" spans="4:4">
-      <c r="D92" s="6"/>
+      <c r="D92" s="8"/>
     </row>
     <row r="93" spans="4:4">
-      <c r="D93" s="6"/>
+      <c r="D93" s="8"/>
     </row>
     <row r="94" spans="4:4">
-      <c r="D94" s="6"/>
+      <c r="D94" s="8"/>
     </row>
     <row r="95" spans="4:4">
-      <c r="D95" s="6"/>
+      <c r="D95" s="8"/>
     </row>
     <row r="96" spans="4:4">
-      <c r="D96" s="6"/>
+      <c r="D96" s="8"/>
     </row>
     <row r="97" spans="4:4">
-      <c r="D97" s="6"/>
+      <c r="D97" s="8"/>
     </row>
     <row r="98" spans="4:4">
-      <c r="D98" s="6"/>
+      <c r="D98" s="8"/>
     </row>
     <row r="99" spans="4:4">
-      <c r="D99" s="6"/>
+      <c r="D99" s="8"/>
     </row>
     <row r="100" spans="4:4">
-      <c r="D100" s="6"/>
+      <c r="D100" s="8"/>
     </row>
     <row r="101" spans="4:4">
-      <c r="D101" s="6"/>
+      <c r="D101" s="8"/>
     </row>
     <row r="102" spans="4:4">
-      <c r="D102" s="6"/>
+      <c r="D102" s="8"/>
     </row>
     <row r="103" spans="4:4">
-      <c r="D103" s="6"/>
+      <c r="D103" s="8"/>
     </row>
     <row r="104" spans="4:4">
-      <c r="D104" s="6"/>
+      <c r="D104" s="8"/>
     </row>
     <row r="105" spans="4:4">
-      <c r="D105" s="6"/>
+      <c r="D105" s="8"/>
     </row>
     <row r="106" spans="4:4">
-      <c r="D106" s="6"/>
+      <c r="D106" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>